<commit_message>
Add fixtures for DB (for app employees and all DB).
</commit_message>
<xml_diff>
--- a/backend/tempr_data/training_requests.xlsx
+++ b/backend/tempr_data/training_requests.xlsx
@@ -13,7 +13,7 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="54"><si><t>номер заявки</t></si><si><t>id</t></si><si><r><t/></r><r><rPr><b/><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>навык</t></r></si><si><t>Название</t></si><si><t>тикет откуда</t></si><si><t>дата</t></si><si><t>дата закрытия</t></si><si><r><t/></r><r><rPr><b/><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>ответственный</t></r></si><si><r><t/></r><r><rPr><b/><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>Примечание</t></r></si><si><t>Статус</t></si><si><t>Часов_факт</t></si><si><t>Часов_план</t></si><si><t>MacOS</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>работник</t></r></si><si><t>наставник</t></si><si><t>повышение в должности</t></si><si><t>в процессе</t></si><si><t>Pandas</t></si><si><t>работник</t></si><si><t>Повышение в должности, 1400руб, https://stepik.org/course/120014/promo</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Креативное мышление</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>руководитель</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Принятие решения</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Решение проблем</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Управление проектом</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Эмоциональный интеллект</t></r></si><si><t>руководитель</t></si><si><t>Windows</t></si><si><t>на согласовании</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Trello</t></r></si><si><t>одобрено</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Навыки работы с технической документацией и разрешением технических проблем у пользователей.</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Делегирование</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Seaborn</t></r></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Python</t></r></si><si><t>саморазвитие, 3200руб, https://stepik.org/course/82541</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Управление проектом</t></r></si><si><r><t/></r><r><rPr><sz val="9"/><color rgb="FF1f1f1f"/><rFont val="&quot" /><family val="2"/></rPr><t>саморазвитие</t></r></si><si><t>отмена</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Межличностные навыки</t></r></si><si><t>HR</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Ораторское искусство</t></r></si><si><t>Нет данных</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Linux</t></r></si><si><t>регулярная</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Jira</t></r></si><si><t>для нового проекта</t></si><si><t>отказано</t></si><si><t>CorelDraw</t></si><si><t>PhotoShop</t></si><si><t>Linux</t></si><si><t>Asana</t></si><si><t>Jira</t></si><si><t>Trello</t></si></sst>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?><sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="57"><si><t>номер заявки</t></si><si><t>сотрудник</t></si><si><r><t/></r><r><rPr><b/><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>навык</t></r></si><si><t>Название</t></si><si><t>тикет откуда</t></si><si><t>дата</t></si><si><t>дата закрытия</t></si><si><r><t/></r><r><rPr><b/><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>ответственный</t></r></si><si><r><t/></r><r><rPr><b/><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>Примечание</t></r></si><si><t>Статус</t></si><si><t>Часов_факт</t></si><si><t>Часов_план</t></si><si><t>Скворцова Мария</t></si><si><t>MacOS</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>работник</t></r></si><si><t>наставник</t></si><si><t>повышение в должности</t></si><si><t>в процессе</t></si><si><t>Pandas</t></si><si><t>работник</t></si><si><t>Повышение в должности, 1400руб, https://stepik.org/course/120014/promo</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Креативное мышление</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF1f1f1f"/><rFont val="Arial" /><family val="2"/></rPr><t>руководитель</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Принятие решения</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Решение проблем</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Управление проектом</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Эмоциональный интеллект</t></r></si><si><t>руководитель</t></si><si><t>Windows</t></si><si><t>на согласовании</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Trello</t></r></si><si><t>одобрено</t></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Навыки работы с технической документацией и разрешением технических проблем у пользователей.</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Делегирование</t></r></si><si><r><t/></r><r><rPr><sz val="10"/><color rgb="FF212121"/><rFont val="Arial" /><family val="2"/></rPr><t>Seaborn</t></r></si><si><t>Смирнова Милана</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Python</t></r></si><si><t>саморазвитие, 3200руб, https://stepik.org/course/82541</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Управление проектом</t></r></si><si><r><t/></r><r><rPr><sz val="9"/><color rgb="FF1f1f1f"/><rFont val="&quot" /><family val="2"/></rPr><t>саморазвитие</t></r></si><si><t>отмена</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Межличностные навыки</t></r></si><si><t>HR</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Ораторское искусство</t></r></si><si><t>Нет данных</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Linux</t></r></si><si><t>регулярная</t></si><si><r><t/></r><r><rPr><sz val="11"/><color rgb="FF212121"/><rFont val="Roboto" /><family val="2"/></rPr><t>Jira</t></r></si><si><t>для нового проекта</t></si><si><t>отказано</t></si><si><t>Волкова Ксения</t></si><si><t>CorelDraw</t></si><si><t>PhotoShop</t></si><si><t>Linux</t></si><si><t>Asana</t></si><si><t>Jira</t></si><si><t>Trello</t></si></sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,7 +520,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="20" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="21" width="11.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="21" width="29.290714285714284" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="22" width="57.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="21" width="11.862142857142858" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="23" width="11.862142857142858" customWidth="1" bestFit="1"/>
@@ -575,17 +575,17 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="6">
-        <v>4</v>
+      <c r="B2" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8">
         <v>5</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="10">
         <v>45510</v>
@@ -594,13 +594,13 @@
         <v>45571</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="11">
         <v>42</v>
@@ -613,17 +613,17 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="6">
-        <v>4</v>
+      <c r="B3" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="8">
         <v>5</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F3" s="10">
         <v>45510</v>
@@ -632,13 +632,13 @@
         <v>45571</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K3" s="11">
         <v>42</v>
@@ -651,17 +651,17 @@
       <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B4" s="6">
-        <v>4</v>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="8">
         <v>5</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="10">
         <v>45510</v>
@@ -670,13 +670,13 @@
         <v>45572</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K4" s="11">
         <v>40</v>
@@ -689,17 +689,17 @@
       <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
-        <v>4</v>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="8">
         <v>5</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" s="10">
         <v>45510</v>
@@ -708,13 +708,13 @@
         <v>45573</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K5" s="11">
         <v>15</v>
@@ -727,17 +727,17 @@
       <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
-        <v>4</v>
+      <c r="B6" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="8">
         <v>5</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="10">
         <v>45510</v>
@@ -746,13 +746,13 @@
         <v>45574</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K6" s="11">
         <v>15</v>
@@ -765,17 +765,17 @@
       <c r="A7" s="6">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
-        <v>4</v>
+      <c r="B7" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="8">
         <v>5</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F7" s="10">
         <v>45510</v>
@@ -784,13 +784,13 @@
         <v>45575</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I7" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K7" s="11">
         <v>20</v>
@@ -803,17 +803,17 @@
       <c r="A8" s="6">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
-        <v>4</v>
+      <c r="B8" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="8">
         <v>5</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F8" s="10">
         <v>45510</v>
@@ -822,13 +822,13 @@
         <v>45576</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K8" s="11">
         <v>10</v>
@@ -841,30 +841,30 @@
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
-        <v>4</v>
+      <c r="B9" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="8">
         <v>5</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F9" s="10">
         <v>45510</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I9" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K9" s="11">
         <v>0</v>
@@ -877,17 +877,17 @@
       <c r="A10" s="6">
         <v>9</v>
       </c>
-      <c r="B10" s="6">
-        <v>4</v>
+      <c r="B10" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D10" s="8">
         <v>5</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F10" s="10">
         <v>45510</v>
@@ -896,13 +896,13 @@
         <v>45571</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K10" s="11">
         <v>0</v>
@@ -915,30 +915,30 @@
       <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="B11" s="6">
-        <v>4</v>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D11" s="8">
         <v>5</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F11" s="10">
         <v>45510</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K11" s="11">
         <v>0</v>
@@ -951,30 +951,30 @@
       <c r="A12" s="6">
         <v>11</v>
       </c>
-      <c r="B12" s="6">
-        <v>4</v>
+      <c r="B12" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D12" s="8">
         <v>5</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F12" s="10">
         <v>45510</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K12" s="11">
         <v>0</v>
@@ -987,17 +987,17 @@
       <c r="A13" s="6">
         <v>12</v>
       </c>
-      <c r="B13" s="6">
-        <v>4</v>
+      <c r="B13" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D13" s="8">
         <v>5</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F13" s="10">
         <v>45510</v>
@@ -1006,13 +1006,13 @@
         <v>45571</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K13" s="11">
         <v>0</v>
@@ -1025,17 +1025,17 @@
       <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14" s="11">
-        <v>10</v>
+      <c r="B14" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" s="11">
         <v>4</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F14" s="15">
         <v>45511</v>
@@ -1044,13 +1044,13 @@
         <v>45876</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I14" s="16" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K14" s="11">
         <v>0</v>
@@ -1063,30 +1063,30 @@
       <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15" s="11">
-        <v>10</v>
+      <c r="B15" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D15" s="11">
         <v>5</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F15" s="15">
         <v>45512</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I15" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K15" s="11">
         <v>0</v>
@@ -1099,30 +1099,30 @@
       <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
-        <v>10</v>
+      <c r="B16" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D16" s="11">
         <v>5</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F16" s="15">
         <v>45513</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K16" s="11">
         <v>0</v>
@@ -1135,17 +1135,17 @@
       <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17" s="11">
-        <v>10</v>
+      <c r="B17" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D17" s="11">
         <v>4</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F17" s="15">
         <v>45514</v>
@@ -1154,13 +1154,13 @@
         <v>45545</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I17" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K17" s="11">
         <v>0</v>
@@ -1173,17 +1173,17 @@
       <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
-        <v>10</v>
+      <c r="B18" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D18" s="11">
         <v>5</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F18" s="17">
         <v>45508</v>
@@ -1192,13 +1192,13 @@
         <v>45509</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K18" s="11">
         <v>0</v>
@@ -1211,17 +1211,17 @@
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="11">
-        <v>10</v>
+      <c r="B19" s="11" t="s">
+        <v>35</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D19" s="11">
         <v>4</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F19" s="15">
         <v>45512</v>
@@ -1230,13 +1230,13 @@
         <v>45543</v>
       </c>
       <c r="H19" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="K19" s="11">
         <v>0</v>
@@ -1249,17 +1249,17 @@
       <c r="A20" s="6">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
-        <v>77</v>
+      <c r="B20" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D20" s="18">
         <v>4</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F20" s="17">
         <v>45505</v>
@@ -1268,13 +1268,13 @@
         <v>45509</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K20" s="11">
         <v>0</v>
@@ -1287,17 +1287,17 @@
       <c r="A21" s="6">
         <v>20</v>
       </c>
-      <c r="B21" s="11">
-        <v>77</v>
+      <c r="B21" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D21" s="18">
         <v>5</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F21" s="19">
         <v>45505</v>
@@ -1306,13 +1306,13 @@
         <v>45509</v>
       </c>
       <c r="H21" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K21" s="11">
         <v>5</v>
@@ -1325,17 +1325,17 @@
       <c r="A22" s="6">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
-        <v>77</v>
+      <c r="B22" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D22" s="18">
         <v>5</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F22" s="17">
         <v>45505</v>
@@ -1344,13 +1344,13 @@
         <v>45509</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K22" s="11">
         <v>30</v>
@@ -1363,17 +1363,17 @@
       <c r="A23" s="6">
         <v>22</v>
       </c>
-      <c r="B23" s="11">
-        <v>77</v>
+      <c r="B23" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="18">
         <v>5</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F23" s="19">
         <v>45505</v>
@@ -1382,13 +1382,13 @@
         <v>45509</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K23" s="11">
         <v>15</v>
@@ -1401,17 +1401,17 @@
       <c r="A24" s="6">
         <v>23</v>
       </c>
-      <c r="B24" s="11">
-        <v>77</v>
+      <c r="B24" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="18">
         <v>5</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F24" s="17">
         <v>45505</v>
@@ -1420,13 +1420,13 @@
         <v>45509</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K24" s="11">
         <v>2</v>
@@ -1439,17 +1439,17 @@
       <c r="A25" s="6">
         <v>24</v>
       </c>
-      <c r="B25" s="11">
-        <v>77</v>
+      <c r="B25" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D25" s="18">
         <v>5</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F25" s="19">
         <v>45505</v>
@@ -1458,13 +1458,13 @@
         <v>45509</v>
       </c>
       <c r="H25" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K25" s="11">
         <v>12</v>
@@ -1477,17 +1477,17 @@
       <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26" s="11">
-        <v>77</v>
+      <c r="B26" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D26" s="18">
         <v>5</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F26" s="17">
         <v>45505</v>
@@ -1496,13 +1496,13 @@
         <v>45509</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K26" s="11">
         <v>0</v>
@@ -1515,17 +1515,17 @@
       <c r="A27" s="6">
         <v>26</v>
       </c>
-      <c r="B27" s="11">
-        <v>77</v>
+      <c r="B27" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D27" s="18">
         <v>4</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F27" s="19">
         <v>45505</v>
@@ -1534,13 +1534,13 @@
         <v>45509</v>
       </c>
       <c r="H27" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K27" s="11">
         <v>0</v>

</xml_diff>